<commit_message>
RDM-5519: Added a test case to verify the correct security classification for each caseType
</commit_message>
<xml_diff>
--- a/aat/src/resource/CCD_CNP_27_CaseType_Security_Classification_Test.xlsx
+++ b/aat/src/resource/CCD_CNP_27_CaseType_Security_Classification_Test.xlsx
@@ -5,11 +5,11 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CCD AM Integration\ccd-definition-store\aat\src\resource\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CCD AM Integration\ccd-docker\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1080" windowWidth="29180" windowHeight="16620" tabRatio="823" firstSheet="1" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="1080" windowWidth="29180" windowHeight="16620" tabRatio="823" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2636" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2650" uniqueCount="281">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -896,13 +896,13 @@
     <t>AUTOTEST2</t>
   </si>
   <si>
-    <t>caseworker-AUTOTEST2</t>
-  </si>
-  <si>
     <t>Auto Test 2</t>
   </si>
   <si>
     <t>RESTRICTED</t>
+  </si>
+  <si>
+    <t>caseworker-autotest2</t>
   </si>
 </sst>
 </file>
@@ -1834,7 +1834,7 @@
         <v>277</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>24</v>
@@ -1863,7 +1863,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -3979,7 +3979,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.36328125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4044,7 +4044,7 @@
         <v>274</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="E4" s="14" t="s">
         <v>124</v>
@@ -4059,7 +4059,7 @@
         <v>275</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="E5" s="14" t="s">
         <v>124</v>
@@ -4074,7 +4074,7 @@
         <v>276</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="E6" s="14" t="s">
         <v>124</v>
@@ -4174,7 +4174,7 @@
         <v>184</v>
       </c>
       <c r="E4" s="60" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="F4" s="74" t="s">
         <v>124</v>
@@ -4192,7 +4192,7 @@
         <v>185</v>
       </c>
       <c r="E5" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="F5" s="74" t="s">
         <v>124</v>
@@ -4210,7 +4210,7 @@
         <v>188</v>
       </c>
       <c r="E6" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="F6" s="74" t="s">
         <v>124</v>
@@ -4228,7 +4228,7 @@
         <v>184</v>
       </c>
       <c r="E7" s="60" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="F7" s="74" t="s">
         <v>124</v>
@@ -4246,7 +4246,7 @@
         <v>185</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="F8" s="74" t="s">
         <v>124</v>
@@ -4264,7 +4264,7 @@
         <v>188</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="F9" s="74" t="s">
         <v>124</v>
@@ -4282,7 +4282,7 @@
         <v>184</v>
       </c>
       <c r="E10" s="60" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="F10" s="74" t="s">
         <v>124</v>
@@ -4300,7 +4300,7 @@
         <v>185</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="F11" s="74" t="s">
         <v>124</v>
@@ -4318,7 +4318,7 @@
         <v>188</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="F12" s="74" t="s">
         <v>124</v>
@@ -4415,7 +4415,7 @@
         <v>189</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="F4" s="24" t="s">
         <v>124</v>
@@ -4432,7 +4432,7 @@
         <v>191</v>
       </c>
       <c r="E5" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="F5" s="24" t="s">
         <v>124</v>
@@ -4449,7 +4449,7 @@
         <v>193</v>
       </c>
       <c r="E6" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="F6" s="24" t="s">
         <v>124</v>
@@ -4466,7 +4466,7 @@
         <v>195</v>
       </c>
       <c r="E7" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="F7" s="24" t="s">
         <v>124</v>
@@ -4483,7 +4483,7 @@
         <v>197</v>
       </c>
       <c r="E8" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="F8" s="24" t="s">
         <v>124</v>
@@ -4500,7 +4500,7 @@
         <v>205</v>
       </c>
       <c r="E9" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="F9" s="24" t="s">
         <v>124</v>
@@ -4517,7 +4517,7 @@
         <v>189</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="F10" s="24" t="s">
         <v>124</v>
@@ -4534,7 +4534,7 @@
         <v>191</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="F11" s="24" t="s">
         <v>124</v>
@@ -4551,7 +4551,7 @@
         <v>193</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="F12" s="24" t="s">
         <v>124</v>
@@ -4568,7 +4568,7 @@
         <v>195</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="F13" s="24" t="s">
         <v>124</v>
@@ -4585,7 +4585,7 @@
         <v>197</v>
       </c>
       <c r="E14" s="14" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="F14" s="24" t="s">
         <v>124</v>
@@ -4602,7 +4602,7 @@
         <v>205</v>
       </c>
       <c r="E15" s="14" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="F15" s="24" t="s">
         <v>124</v>
@@ -4620,7 +4620,7 @@
         <v>189</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="F16" s="24" t="s">
         <v>124</v>
@@ -4638,7 +4638,7 @@
         <v>191</v>
       </c>
       <c r="E17" s="14" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="F17" s="24" t="s">
         <v>124</v>
@@ -4656,7 +4656,7 @@
         <v>193</v>
       </c>
       <c r="E18" s="14" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="F18" s="24" t="s">
         <v>124</v>
@@ -4674,7 +4674,7 @@
         <v>195</v>
       </c>
       <c r="E19" s="14" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="F19" s="24" t="s">
         <v>124</v>
@@ -4692,7 +4692,7 @@
         <v>197</v>
       </c>
       <c r="E20" s="14" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="F20" s="24" t="s">
         <v>124</v>
@@ -4710,7 +4710,7 @@
         <v>205</v>
       </c>
       <c r="E21" s="14" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="F21" s="24" t="s">
         <v>124</v>
@@ -4731,8 +4731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F53"/>
   <sheetViews>
-    <sheetView topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38:C53"/>
+    <sheetView topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.36328125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4806,7 +4806,7 @@
         <v>134</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="F4" s="24" t="s">
         <v>124</v>
@@ -4823,7 +4823,7 @@
         <v>136</v>
       </c>
       <c r="E5" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="F5" s="24" t="s">
         <v>124</v>
@@ -4840,7 +4840,7 @@
         <v>138</v>
       </c>
       <c r="E6" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="F6" s="24" t="s">
         <v>124</v>
@@ -4857,7 +4857,7 @@
         <v>143</v>
       </c>
       <c r="E7" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="F7" s="24" t="s">
         <v>124</v>
@@ -4874,7 +4874,7 @@
         <v>145</v>
       </c>
       <c r="E8" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="F8" s="24" t="s">
         <v>124</v>
@@ -4891,7 +4891,7 @@
         <v>149</v>
       </c>
       <c r="E9" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="F9" s="24" t="s">
         <v>124</v>
@@ -4908,7 +4908,7 @@
         <v>157</v>
       </c>
       <c r="E10" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="F10" s="24" t="s">
         <v>124</v>
@@ -4925,7 +4925,7 @@
         <v>242</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="F11" s="24" t="s">
         <v>124</v>
@@ -4942,7 +4942,7 @@
         <v>155</v>
       </c>
       <c r="E12" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="F12" s="24" t="s">
         <v>124</v>
@@ -4959,7 +4959,7 @@
         <v>159</v>
       </c>
       <c r="E13" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="F13" s="24" t="s">
         <v>124</v>
@@ -4976,7 +4976,7 @@
         <v>169</v>
       </c>
       <c r="E14" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="F14" s="24" t="s">
         <v>124</v>
@@ -4993,7 +4993,7 @@
         <v>238</v>
       </c>
       <c r="E15" s="14" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="F15" s="24" t="s">
         <v>124</v>
@@ -5011,7 +5011,7 @@
         <v>235</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="F16" s="24" t="s">
         <v>124</v>
@@ -5028,7 +5028,7 @@
         <v>224</v>
       </c>
       <c r="E17" s="14" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="F17" s="24" t="s">
         <v>124</v>
@@ -5046,7 +5046,7 @@
         <v>246</v>
       </c>
       <c r="E18" s="14" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="F18" s="24" t="s">
         <v>124</v>
@@ -5063,7 +5063,7 @@
         <v>250</v>
       </c>
       <c r="E19" s="14" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="F19" s="24" t="s">
         <v>124</v>
@@ -5080,7 +5080,7 @@
         <v>261</v>
       </c>
       <c r="E20" s="14" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="F20" s="24" t="s">
         <v>124</v>
@@ -5097,7 +5097,7 @@
         <v>134</v>
       </c>
       <c r="E21" s="14" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="F21" s="24" t="s">
         <v>124</v>
@@ -5114,7 +5114,7 @@
         <v>136</v>
       </c>
       <c r="E22" s="14" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="F22" s="24" t="s">
         <v>124</v>
@@ -5131,7 +5131,7 @@
         <v>138</v>
       </c>
       <c r="E23" s="14" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="F23" s="24" t="s">
         <v>124</v>
@@ -5148,7 +5148,7 @@
         <v>143</v>
       </c>
       <c r="E24" s="14" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="F24" s="24" t="s">
         <v>124</v>
@@ -5165,7 +5165,7 @@
         <v>145</v>
       </c>
       <c r="E25" s="14" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="F25" s="24" t="s">
         <v>124</v>
@@ -5182,7 +5182,7 @@
         <v>149</v>
       </c>
       <c r="E26" s="14" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="F26" s="24" t="s">
         <v>124</v>
@@ -5199,7 +5199,7 @@
         <v>157</v>
       </c>
       <c r="E27" s="14" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="F27" s="24" t="s">
         <v>124</v>
@@ -5216,7 +5216,7 @@
         <v>242</v>
       </c>
       <c r="E28" s="14" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="F28" s="24" t="s">
         <v>124</v>
@@ -5233,7 +5233,7 @@
         <v>155</v>
       </c>
       <c r="E29" s="14" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="F29" s="24" t="s">
         <v>124</v>
@@ -5250,7 +5250,7 @@
         <v>159</v>
       </c>
       <c r="E30" s="14" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="F30" s="24" t="s">
         <v>124</v>
@@ -5267,7 +5267,7 @@
         <v>169</v>
       </c>
       <c r="E31" s="14" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="F31" s="24" t="s">
         <v>124</v>
@@ -5284,7 +5284,7 @@
         <v>238</v>
       </c>
       <c r="E32" s="14" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="F32" s="24" t="s">
         <v>124</v>
@@ -5301,7 +5301,7 @@
         <v>235</v>
       </c>
       <c r="E33" s="14" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="F33" s="24" t="s">
         <v>124</v>
@@ -5318,7 +5318,7 @@
         <v>224</v>
       </c>
       <c r="E34" s="14" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="F34" s="24" t="s">
         <v>124</v>
@@ -5335,7 +5335,7 @@
         <v>250</v>
       </c>
       <c r="E35" s="14" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="F35" s="24" t="s">
         <v>124</v>
@@ -5352,7 +5352,7 @@
         <v>261</v>
       </c>
       <c r="E36" s="14" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="F36" s="24" t="s">
         <v>124</v>
@@ -5370,7 +5370,7 @@
         <v>134</v>
       </c>
       <c r="E37" s="14" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="F37" s="24" t="s">
         <v>124</v>
@@ -5388,7 +5388,7 @@
         <v>136</v>
       </c>
       <c r="E38" s="14" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="F38" s="24" t="s">
         <v>124</v>
@@ -5406,7 +5406,7 @@
         <v>138</v>
       </c>
       <c r="E39" s="14" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="F39" s="24" t="s">
         <v>124</v>
@@ -5424,7 +5424,7 @@
         <v>143</v>
       </c>
       <c r="E40" s="14" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="F40" s="24" t="s">
         <v>124</v>
@@ -5442,7 +5442,7 @@
         <v>145</v>
       </c>
       <c r="E41" s="14" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="F41" s="24" t="s">
         <v>124</v>
@@ -5460,7 +5460,7 @@
         <v>149</v>
       </c>
       <c r="E42" s="14" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="F42" s="24" t="s">
         <v>124</v>
@@ -5478,7 +5478,7 @@
         <v>157</v>
       </c>
       <c r="E43" s="14" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="F43" s="24" t="s">
         <v>124</v>
@@ -5496,7 +5496,7 @@
         <v>242</v>
       </c>
       <c r="E44" s="14" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="F44" s="24" t="s">
         <v>124</v>
@@ -5514,7 +5514,7 @@
         <v>155</v>
       </c>
       <c r="E45" s="14" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="F45" s="24" t="s">
         <v>124</v>
@@ -5532,7 +5532,7 @@
         <v>159</v>
       </c>
       <c r="E46" s="14" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="F46" s="24" t="s">
         <v>124</v>
@@ -5550,7 +5550,7 @@
         <v>169</v>
       </c>
       <c r="E47" s="14" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="F47" s="24" t="s">
         <v>124</v>
@@ -5568,7 +5568,7 @@
         <v>238</v>
       </c>
       <c r="E48" s="14" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="F48" s="24" t="s">
         <v>124</v>
@@ -5586,7 +5586,7 @@
         <v>235</v>
       </c>
       <c r="E49" s="14" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="F49" s="24" t="s">
         <v>124</v>
@@ -5604,7 +5604,7 @@
         <v>224</v>
       </c>
       <c r="E50" s="14" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="F50" s="24" t="s">
         <v>124</v>
@@ -5622,7 +5622,7 @@
         <v>246</v>
       </c>
       <c r="E51" s="14" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="F51" s="24" t="s">
         <v>124</v>
@@ -5640,7 +5640,7 @@
         <v>250</v>
       </c>
       <c r="E52" s="14" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="F52" s="24" t="s">
         <v>124</v>
@@ -5658,7 +5658,7 @@
         <v>261</v>
       </c>
       <c r="E53" s="14" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="F53" s="24" t="s">
         <v>124</v>
@@ -5768,7 +5768,7 @@
         <v>214</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="G4" s="81" t="s">
         <v>124</v>
@@ -5788,7 +5788,7 @@
         <v>216</v>
       </c>
       <c r="F5" s="14" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="G5" s="81" t="s">
         <v>124</v>
@@ -5808,7 +5808,7 @@
         <v>222</v>
       </c>
       <c r="F6" s="14" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="G6" s="81" t="s">
         <v>124</v>
@@ -5828,7 +5828,7 @@
         <v>214</v>
       </c>
       <c r="F7" s="14" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="G7" s="81" t="s">
         <v>124</v>
@@ -5848,7 +5848,7 @@
         <v>216</v>
       </c>
       <c r="F8" s="14" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="G8" s="81" t="s">
         <v>124</v>
@@ -5868,7 +5868,7 @@
         <v>222</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="G9" s="81" t="s">
         <v>124</v>
@@ -5888,7 +5888,7 @@
         <v>214</v>
       </c>
       <c r="F10" s="14" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="G10" s="81" t="s">
         <v>124</v>
@@ -5908,7 +5908,7 @@
         <v>216</v>
       </c>
       <c r="F11" s="14" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="G11" s="81" t="s">
         <v>124</v>
@@ -5928,7 +5928,7 @@
         <v>222</v>
       </c>
       <c r="F12" s="14" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="G12" s="81" t="s">
         <v>124</v>
@@ -5944,7 +5944,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
@@ -6096,7 +6096,7 @@
       <c r="G6" s="14"/>
       <c r="H6" s="14"/>
       <c r="I6" s="14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
   </sheetData>
@@ -6120,10 +6120,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M52"/>
+  <dimension ref="A1:M54"/>
   <sheetViews>
-    <sheetView topLeftCell="G34" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="K37" sqref="K37:K52"/>
+    <sheetView topLeftCell="G36" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="K39" sqref="K39:K54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.36328125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -7090,7 +7090,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="33" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="13">
         <v>42736</v>
       </c>
@@ -7119,7 +7119,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="34" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="13">
         <v>42736</v>
       </c>
@@ -7148,7 +7148,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="35" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="13">
         <v>42736</v>
       </c>
@@ -7157,20 +7157,18 @@
         <v>275</v>
       </c>
       <c r="D35" s="42" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="E35" s="42" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="F35" s="42" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="G35" s="42" t="s">
-        <v>253</v>
-      </c>
-      <c r="H35" s="42" t="s">
-        <v>254</v>
-      </c>
+        <v>249</v>
+      </c>
+      <c r="H35" s="42"/>
       <c r="I35" s="28" t="s">
         <v>26</v>
       </c>
@@ -7179,7 +7177,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="36" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="13">
         <v>42736</v>
       </c>
@@ -7188,18 +7186,20 @@
         <v>275</v>
       </c>
       <c r="D36" s="42" t="s">
-        <v>261</v>
+        <v>250</v>
       </c>
       <c r="E36" s="42" t="s">
-        <v>262</v>
+        <v>251</v>
       </c>
       <c r="F36" s="42" t="s">
-        <v>263</v>
-      </c>
-      <c r="G36" s="75" t="s">
-        <v>264</v>
-      </c>
-      <c r="H36" s="42"/>
+        <v>252</v>
+      </c>
+      <c r="G36" s="42" t="s">
+        <v>253</v>
+      </c>
+      <c r="H36" s="42" t="s">
+        <v>254</v>
+      </c>
       <c r="I36" s="28" t="s">
         <v>26</v>
       </c>
@@ -7208,36 +7208,38 @@
         <v>273</v>
       </c>
     </row>
-    <row r="37" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="13">
         <v>42736</v>
       </c>
       <c r="B37" s="13"/>
       <c r="C37" s="28" t="s">
-        <v>276</v>
-      </c>
-      <c r="D37" s="28" t="s">
-        <v>134</v>
-      </c>
-      <c r="E37" s="28" t="s">
-        <v>135</v>
-      </c>
-      <c r="F37" s="28" t="s">
-        <v>142</v>
-      </c>
-      <c r="G37" s="28" t="s">
-        <v>25</v>
-      </c>
-      <c r="H37" s="28"/>
+        <v>275</v>
+      </c>
+      <c r="D37" s="42" t="s">
+        <v>261</v>
+      </c>
+      <c r="E37" s="42" t="s">
+        <v>262</v>
+      </c>
+      <c r="F37" s="42" t="s">
+        <v>263</v>
+      </c>
+      <c r="G37" s="75" t="s">
+        <v>264</v>
+      </c>
+      <c r="H37" s="42"/>
       <c r="I37" s="28" t="s">
         <v>26</v>
       </c>
       <c r="J37" s="28"/>
       <c r="K37" s="28" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>273</v>
+      </c>
+      <c r="L37" s="14"/>
+      <c r="M37" s="14"/>
+    </row>
+    <row r="38" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="13">
         <v>42736</v>
       </c>
@@ -7246,16 +7248,16 @@
         <v>276</v>
       </c>
       <c r="D38" s="28" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E38" s="28" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="F38" s="28" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="G38" s="28" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="H38" s="28"/>
       <c r="I38" s="28" t="s">
@@ -7263,10 +7265,10 @@
       </c>
       <c r="J38" s="28"/>
       <c r="K38" s="28" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="13">
         <v>42736</v>
       </c>
@@ -7275,16 +7277,16 @@
         <v>276</v>
       </c>
       <c r="D39" s="28" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E39" s="28" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F39" s="28" t="s">
-        <v>140</v>
-      </c>
-      <c r="G39" s="42" t="s">
-        <v>30</v>
+        <v>141</v>
+      </c>
+      <c r="G39" s="28" t="s">
+        <v>28</v>
       </c>
       <c r="H39" s="28"/>
       <c r="I39" s="28" t="s">
@@ -7292,10 +7294,10 @@
       </c>
       <c r="J39" s="28"/>
       <c r="K39" s="28" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="13">
         <v>42736</v>
       </c>
@@ -7303,17 +7305,17 @@
       <c r="C40" s="28" t="s">
         <v>276</v>
       </c>
-      <c r="D40" s="42" t="s">
-        <v>143</v>
-      </c>
-      <c r="E40" s="42" t="s">
-        <v>144</v>
-      </c>
-      <c r="F40" s="42" t="s">
-        <v>147</v>
+      <c r="D40" s="28" t="s">
+        <v>138</v>
+      </c>
+      <c r="E40" s="28" t="s">
+        <v>139</v>
+      </c>
+      <c r="F40" s="28" t="s">
+        <v>140</v>
       </c>
       <c r="G40" s="42" t="s">
-        <v>86</v>
+        <v>30</v>
       </c>
       <c r="H40" s="28"/>
       <c r="I40" s="28" t="s">
@@ -7321,10 +7323,10 @@
       </c>
       <c r="J40" s="28"/>
       <c r="K40" s="28" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="13">
         <v>42736</v>
       </c>
@@ -7333,16 +7335,16 @@
         <v>276</v>
       </c>
       <c r="D41" s="42" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E41" s="42" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F41" s="42" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G41" s="42" t="s">
-        <v>29</v>
+        <v>86</v>
       </c>
       <c r="H41" s="28"/>
       <c r="I41" s="28" t="s">
@@ -7350,10 +7352,10 @@
       </c>
       <c r="J41" s="28"/>
       <c r="K41" s="28" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="13">
         <v>42736</v>
       </c>
@@ -7362,16 +7364,16 @@
         <v>276</v>
       </c>
       <c r="D42" s="42" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="E42" s="42" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="F42" s="42" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="G42" s="42" t="s">
-        <v>85</v>
+        <v>29</v>
       </c>
       <c r="H42" s="28"/>
       <c r="I42" s="28" t="s">
@@ -7379,10 +7381,10 @@
       </c>
       <c r="J42" s="28"/>
       <c r="K42" s="28" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="13">
         <v>42736</v>
       </c>
@@ -7391,16 +7393,16 @@
         <v>276</v>
       </c>
       <c r="D43" s="42" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="E43" s="42" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F43" s="42" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G43" s="42" t="s">
-        <v>27</v>
+        <v>85</v>
       </c>
       <c r="H43" s="28"/>
       <c r="I43" s="28" t="s">
@@ -7408,10 +7410,10 @@
       </c>
       <c r="J43" s="28"/>
       <c r="K43" s="28" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="13">
         <v>42736</v>
       </c>
@@ -7420,16 +7422,16 @@
         <v>276</v>
       </c>
       <c r="D44" s="42" t="s">
-        <v>242</v>
+        <v>157</v>
       </c>
       <c r="E44" s="42" t="s">
-        <v>243</v>
+        <v>152</v>
       </c>
       <c r="F44" s="42" t="s">
-        <v>244</v>
+        <v>153</v>
       </c>
       <c r="G44" s="42" t="s">
-        <v>245</v>
+        <v>27</v>
       </c>
       <c r="H44" s="28"/>
       <c r="I44" s="28" t="s">
@@ -7437,10 +7439,10 @@
       </c>
       <c r="J44" s="28"/>
       <c r="K44" s="28" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="13">
         <v>42736</v>
       </c>
@@ -7449,16 +7451,16 @@
         <v>276</v>
       </c>
       <c r="D45" s="42" t="s">
-        <v>155</v>
+        <v>242</v>
       </c>
       <c r="E45" s="42" t="s">
-        <v>156</v>
+        <v>243</v>
       </c>
       <c r="F45" s="42" t="s">
-        <v>158</v>
+        <v>244</v>
       </c>
       <c r="G45" s="42" t="s">
-        <v>154</v>
+        <v>245</v>
       </c>
       <c r="H45" s="28"/>
       <c r="I45" s="28" t="s">
@@ -7466,10 +7468,10 @@
       </c>
       <c r="J45" s="28"/>
       <c r="K45" s="28" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="13">
         <v>42736</v>
       </c>
@@ -7478,29 +7480,27 @@
         <v>276</v>
       </c>
       <c r="D46" s="42" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="E46" s="42" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="F46" s="42" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="G46" s="42" t="s">
-        <v>31</v>
-      </c>
-      <c r="H46" s="42" t="s">
-        <v>162</v>
-      </c>
+        <v>154</v>
+      </c>
+      <c r="H46" s="28"/>
       <c r="I46" s="28" t="s">
         <v>26</v>
       </c>
       <c r="J46" s="28"/>
       <c r="K46" s="28" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="13">
         <v>42736</v>
       </c>
@@ -7509,29 +7509,29 @@
         <v>276</v>
       </c>
       <c r="D47" s="42" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="E47" s="42" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="F47" s="42" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="G47" s="42" t="s">
-        <v>94</v>
+        <v>31</v>
       </c>
       <c r="H47" s="42" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="I47" s="28" t="s">
         <v>26</v>
       </c>
       <c r="J47" s="28"/>
       <c r="K47" s="28" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="13">
         <v>42736</v>
       </c>
@@ -7540,26 +7540,26 @@
         <v>276</v>
       </c>
       <c r="D48" s="42" t="s">
-        <v>235</v>
+        <v>169</v>
       </c>
       <c r="E48" s="42" t="s">
-        <v>236</v>
+        <v>170</v>
       </c>
       <c r="F48" s="42" t="s">
-        <v>237</v>
+        <v>171</v>
       </c>
       <c r="G48" s="42" t="s">
-        <v>80</v>
+        <v>94</v>
       </c>
       <c r="H48" s="42" t="s">
-        <v>25</v>
+        <v>172</v>
       </c>
       <c r="I48" s="28" t="s">
         <v>26</v>
       </c>
       <c r="J48" s="28"/>
       <c r="K48" s="28" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="49" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7571,24 +7571,26 @@
         <v>276</v>
       </c>
       <c r="D49" s="42" t="s">
-        <v>224</v>
+        <v>235</v>
       </c>
       <c r="E49" s="42" t="s">
-        <v>225</v>
+        <v>236</v>
       </c>
       <c r="F49" s="42" t="s">
-        <v>226</v>
+        <v>237</v>
       </c>
       <c r="G49" s="42" t="s">
-        <v>227</v>
-      </c>
-      <c r="H49" s="42"/>
+        <v>80</v>
+      </c>
+      <c r="H49" s="42" t="s">
+        <v>25</v>
+      </c>
       <c r="I49" s="28" t="s">
         <v>26</v>
       </c>
       <c r="J49" s="28"/>
       <c r="K49" s="28" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="50" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7600,16 +7602,16 @@
         <v>276</v>
       </c>
       <c r="D50" s="42" t="s">
-        <v>238</v>
+        <v>224</v>
       </c>
       <c r="E50" s="42" t="s">
-        <v>239</v>
+        <v>225</v>
       </c>
       <c r="F50" s="42" t="s">
-        <v>240</v>
+        <v>226</v>
       </c>
       <c r="G50" s="42" t="s">
-        <v>241</v>
+        <v>227</v>
       </c>
       <c r="H50" s="42"/>
       <c r="I50" s="28" t="s">
@@ -7617,7 +7619,7 @@
       </c>
       <c r="J50" s="28"/>
       <c r="K50" s="28" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="51" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7629,26 +7631,24 @@
         <v>276</v>
       </c>
       <c r="D51" s="42" t="s">
-        <v>250</v>
+        <v>238</v>
       </c>
       <c r="E51" s="42" t="s">
-        <v>251</v>
+        <v>239</v>
       </c>
       <c r="F51" s="42" t="s">
-        <v>252</v>
+        <v>240</v>
       </c>
       <c r="G51" s="42" t="s">
-        <v>253</v>
-      </c>
-      <c r="H51" s="42" t="s">
-        <v>254</v>
-      </c>
+        <v>241</v>
+      </c>
+      <c r="H51" s="42"/>
       <c r="I51" s="28" t="s">
         <v>26</v>
       </c>
       <c r="J51" s="28"/>
       <c r="K51" s="28" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="52" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7660,16 +7660,16 @@
         <v>276</v>
       </c>
       <c r="D52" s="42" t="s">
-        <v>261</v>
+        <v>246</v>
       </c>
       <c r="E52" s="42" t="s">
-        <v>262</v>
+        <v>247</v>
       </c>
       <c r="F52" s="42" t="s">
-        <v>263</v>
-      </c>
-      <c r="G52" s="75" t="s">
-        <v>264</v>
+        <v>248</v>
+      </c>
+      <c r="G52" s="42" t="s">
+        <v>249</v>
       </c>
       <c r="H52" s="42"/>
       <c r="I52" s="28" t="s">
@@ -7677,15 +7677,75 @@
       </c>
       <c r="J52" s="28"/>
       <c r="K52" s="28" t="s">
-        <v>280</v>
+        <v>279</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="13">
+        <v>42736</v>
+      </c>
+      <c r="B53" s="13"/>
+      <c r="C53" s="28" t="s">
+        <v>276</v>
+      </c>
+      <c r="D53" s="42" t="s">
+        <v>250</v>
+      </c>
+      <c r="E53" s="42" t="s">
+        <v>251</v>
+      </c>
+      <c r="F53" s="42" t="s">
+        <v>252</v>
+      </c>
+      <c r="G53" s="42" t="s">
+        <v>253</v>
+      </c>
+      <c r="H53" s="42" t="s">
+        <v>254</v>
+      </c>
+      <c r="I53" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="J53" s="28"/>
+      <c r="K53" s="28" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="13">
+        <v>42736</v>
+      </c>
+      <c r="B54" s="13"/>
+      <c r="C54" s="28" t="s">
+        <v>276</v>
+      </c>
+      <c r="D54" s="42" t="s">
+        <v>261</v>
+      </c>
+      <c r="E54" s="42" t="s">
+        <v>262</v>
+      </c>
+      <c r="F54" s="42" t="s">
+        <v>263</v>
+      </c>
+      <c r="G54" s="75" t="s">
+        <v>264</v>
+      </c>
+      <c r="H54" s="42"/>
+      <c r="I54" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="J54" s="28"/>
+      <c r="K54" s="28" t="s">
+        <v>279</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A52">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a date on or after 01/01/2017" sqref="A4:A54">
       <formula1>42736</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that after LiveFrom date" sqref="B4:B52">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" prompt="Enter a value that after LiveFrom date" sqref="B4:B54">
       <formula1>IF((DATEDIF(A4,B4,"d")&gt;0),B4)</formula1>
     </dataValidation>
   </dataValidations>
@@ -7948,8 +8008,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N8"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.36328125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -8095,7 +8155,7 @@
         <v>26</v>
       </c>
       <c r="L4" s="42" t="s">
-        <v>117</v>
+        <v>279</v>
       </c>
       <c r="M4" s="35"/>
       <c r="N4" s="8"/>
@@ -8127,7 +8187,7 @@
         <v>26</v>
       </c>
       <c r="L5" s="42" t="s">
-        <v>117</v>
+        <v>279</v>
       </c>
       <c r="M5" s="35"/>
       <c r="N5" s="8"/>
@@ -8157,7 +8217,7 @@
         <v>26</v>
       </c>
       <c r="L6" s="42" t="s">
-        <v>117</v>
+        <v>279</v>
       </c>
     </row>
     <row r="7" spans="1:14" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -8187,7 +8247,7 @@
         <v>26</v>
       </c>
       <c r="L7" s="42" t="s">
-        <v>117</v>
+        <v>279</v>
       </c>
     </row>
     <row r="8" spans="1:14" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -8215,7 +8275,7 @@
         <v>26</v>
       </c>
       <c r="L8" s="42" t="s">
-        <v>117</v>
+        <v>279</v>
       </c>
     </row>
   </sheetData>
@@ -9109,7 +9169,7 @@
         <v>184</v>
       </c>
       <c r="P16" s="14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="Q16" s="24" t="s">
         <v>73</v>
@@ -9140,7 +9200,7 @@
         <v>185</v>
       </c>
       <c r="P17" s="14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="Q17" s="24" t="s">
         <v>73</v>
@@ -9171,7 +9231,7 @@
         <v>184</v>
       </c>
       <c r="P18" s="14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="Q18" s="24" t="s">
         <v>73</v>
@@ -9202,7 +9262,7 @@
         <v>188</v>
       </c>
       <c r="P19" s="14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="Q19" s="24" t="s">
         <v>73</v>
@@ -9233,7 +9293,7 @@
         <v>199</v>
       </c>
       <c r="P20" s="14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="Q20" s="24" t="s">
         <v>73</v>
@@ -9264,7 +9324,7 @@
         <v>199</v>
       </c>
       <c r="P21" s="14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="Q21" s="24" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
RDM-5519: Fixing the build issues.
</commit_message>
<xml_diff>
--- a/aat/src/resource/CCD_CNP_27_CaseType_Security_Classification_Test.xlsx
+++ b/aat/src/resource/CCD_CNP_27_CaseType_Security_Classification_Test.xlsx
@@ -5,11 +5,11 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CCD AM Integration\ccd-docker\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CCD AM Integration\ccd-definition-store\aat\src\resource\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1080" windowWidth="29180" windowHeight="16620" tabRatio="823" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="1080" windowWidth="29180" windowHeight="16620" tabRatio="823" firstSheet="11" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2650" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2650" uniqueCount="280">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -893,16 +893,13 @@
     <t>AATRESTRICTED</t>
   </si>
   <si>
-    <t>AUTOTEST2</t>
-  </si>
-  <si>
-    <t>Auto Test 2</t>
-  </si>
-  <si>
     <t>RESTRICTED</t>
   </si>
   <si>
-    <t>caseworker-autotest2</t>
+    <t>AUTOTEST1</t>
+  </si>
+  <si>
+    <t>caseworker-autotest1</t>
   </si>
 </sst>
 </file>
@@ -1768,7 +1765,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.36328125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1831,9 +1828,9 @@
       </c>
       <c r="B4" s="12"/>
       <c r="C4" s="4" t="s">
-        <v>277</v>
-      </c>
-      <c r="D4" s="4" t="s">
+        <v>278</v>
+      </c>
+      <c r="D4" s="28" t="s">
         <v>278</v>
       </c>
       <c r="E4" s="4" t="s">
@@ -2440,8 +2437,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J52"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38:C52"/>
+    <sheetView topLeftCell="E11" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.36328125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3951,7 +3948,7 @@
         <v>233</v>
       </c>
       <c r="D4" s="28" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="E4" s="28" t="s">
         <v>274</v>
@@ -4044,7 +4041,7 @@
         <v>274</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E4" s="14" t="s">
         <v>124</v>
@@ -4059,7 +4056,7 @@
         <v>275</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E5" s="14" t="s">
         <v>124</v>
@@ -4074,7 +4071,7 @@
         <v>276</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E6" s="14" t="s">
         <v>124</v>
@@ -4095,8 +4092,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -4174,7 +4171,7 @@
         <v>184</v>
       </c>
       <c r="E4" s="60" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F4" s="74" t="s">
         <v>124</v>
@@ -4192,7 +4189,7 @@
         <v>185</v>
       </c>
       <c r="E5" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F5" s="74" t="s">
         <v>124</v>
@@ -4210,7 +4207,7 @@
         <v>188</v>
       </c>
       <c r="E6" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F6" s="74" t="s">
         <v>124</v>
@@ -4228,7 +4225,7 @@
         <v>184</v>
       </c>
       <c r="E7" s="60" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F7" s="74" t="s">
         <v>124</v>
@@ -4246,7 +4243,7 @@
         <v>185</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F8" s="74" t="s">
         <v>124</v>
@@ -4264,7 +4261,7 @@
         <v>188</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F9" s="74" t="s">
         <v>124</v>
@@ -4282,7 +4279,7 @@
         <v>184</v>
       </c>
       <c r="E10" s="60" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F10" s="74" t="s">
         <v>124</v>
@@ -4300,7 +4297,7 @@
         <v>185</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F11" s="74" t="s">
         <v>124</v>
@@ -4318,7 +4315,7 @@
         <v>188</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F12" s="74" t="s">
         <v>124</v>
@@ -4415,7 +4412,7 @@
         <v>189</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F4" s="24" t="s">
         <v>124</v>
@@ -4432,7 +4429,7 @@
         <v>191</v>
       </c>
       <c r="E5" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F5" s="24" t="s">
         <v>124</v>
@@ -4449,7 +4446,7 @@
         <v>193</v>
       </c>
       <c r="E6" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F6" s="24" t="s">
         <v>124</v>
@@ -4466,7 +4463,7 @@
         <v>195</v>
       </c>
       <c r="E7" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F7" s="24" t="s">
         <v>124</v>
@@ -4483,7 +4480,7 @@
         <v>197</v>
       </c>
       <c r="E8" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F8" s="24" t="s">
         <v>124</v>
@@ -4500,7 +4497,7 @@
         <v>205</v>
       </c>
       <c r="E9" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F9" s="24" t="s">
         <v>124</v>
@@ -4517,7 +4514,7 @@
         <v>189</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F10" s="24" t="s">
         <v>124</v>
@@ -4534,7 +4531,7 @@
         <v>191</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F11" s="24" t="s">
         <v>124</v>
@@ -4551,7 +4548,7 @@
         <v>193</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F12" s="24" t="s">
         <v>124</v>
@@ -4568,7 +4565,7 @@
         <v>195</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F13" s="24" t="s">
         <v>124</v>
@@ -4585,7 +4582,7 @@
         <v>197</v>
       </c>
       <c r="E14" s="14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F14" s="24" t="s">
         <v>124</v>
@@ -4602,7 +4599,7 @@
         <v>205</v>
       </c>
       <c r="E15" s="14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F15" s="24" t="s">
         <v>124</v>
@@ -4620,7 +4617,7 @@
         <v>189</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F16" s="24" t="s">
         <v>124</v>
@@ -4638,7 +4635,7 @@
         <v>191</v>
       </c>
       <c r="E17" s="14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F17" s="24" t="s">
         <v>124</v>
@@ -4656,7 +4653,7 @@
         <v>193</v>
       </c>
       <c r="E18" s="14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F18" s="24" t="s">
         <v>124</v>
@@ -4674,7 +4671,7 @@
         <v>195</v>
       </c>
       <c r="E19" s="14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F19" s="24" t="s">
         <v>124</v>
@@ -4692,7 +4689,7 @@
         <v>197</v>
       </c>
       <c r="E20" s="14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F20" s="24" t="s">
         <v>124</v>
@@ -4710,7 +4707,7 @@
         <v>205</v>
       </c>
       <c r="E21" s="14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F21" s="24" t="s">
         <v>124</v>
@@ -4806,7 +4803,7 @@
         <v>134</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F4" s="24" t="s">
         <v>124</v>
@@ -4823,7 +4820,7 @@
         <v>136</v>
       </c>
       <c r="E5" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F5" s="24" t="s">
         <v>124</v>
@@ -4840,7 +4837,7 @@
         <v>138</v>
       </c>
       <c r="E6" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F6" s="24" t="s">
         <v>124</v>
@@ -4857,7 +4854,7 @@
         <v>143</v>
       </c>
       <c r="E7" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F7" s="24" t="s">
         <v>124</v>
@@ -4874,7 +4871,7 @@
         <v>145</v>
       </c>
       <c r="E8" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F8" s="24" t="s">
         <v>124</v>
@@ -4891,7 +4888,7 @@
         <v>149</v>
       </c>
       <c r="E9" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F9" s="24" t="s">
         <v>124</v>
@@ -4908,7 +4905,7 @@
         <v>157</v>
       </c>
       <c r="E10" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F10" s="24" t="s">
         <v>124</v>
@@ -4925,7 +4922,7 @@
         <v>242</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F11" s="24" t="s">
         <v>124</v>
@@ -4942,7 +4939,7 @@
         <v>155</v>
       </c>
       <c r="E12" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F12" s="24" t="s">
         <v>124</v>
@@ -4959,7 +4956,7 @@
         <v>159</v>
       </c>
       <c r="E13" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F13" s="24" t="s">
         <v>124</v>
@@ -4976,7 +4973,7 @@
         <v>169</v>
       </c>
       <c r="E14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F14" s="24" t="s">
         <v>124</v>
@@ -4993,7 +4990,7 @@
         <v>238</v>
       </c>
       <c r="E15" s="14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F15" s="24" t="s">
         <v>124</v>
@@ -5011,7 +5008,7 @@
         <v>235</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F16" s="24" t="s">
         <v>124</v>
@@ -5028,7 +5025,7 @@
         <v>224</v>
       </c>
       <c r="E17" s="14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F17" s="24" t="s">
         <v>124</v>
@@ -5046,7 +5043,7 @@
         <v>246</v>
       </c>
       <c r="E18" s="14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F18" s="24" t="s">
         <v>124</v>
@@ -5063,7 +5060,7 @@
         <v>250</v>
       </c>
       <c r="E19" s="14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F19" s="24" t="s">
         <v>124</v>
@@ -5080,7 +5077,7 @@
         <v>261</v>
       </c>
       <c r="E20" s="14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F20" s="24" t="s">
         <v>124</v>
@@ -5097,7 +5094,7 @@
         <v>134</v>
       </c>
       <c r="E21" s="14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F21" s="24" t="s">
         <v>124</v>
@@ -5114,7 +5111,7 @@
         <v>136</v>
       </c>
       <c r="E22" s="14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F22" s="24" t="s">
         <v>124</v>
@@ -5131,7 +5128,7 @@
         <v>138</v>
       </c>
       <c r="E23" s="14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F23" s="24" t="s">
         <v>124</v>
@@ -5148,7 +5145,7 @@
         <v>143</v>
       </c>
       <c r="E24" s="14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F24" s="24" t="s">
         <v>124</v>
@@ -5165,7 +5162,7 @@
         <v>145</v>
       </c>
       <c r="E25" s="14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F25" s="24" t="s">
         <v>124</v>
@@ -5182,7 +5179,7 @@
         <v>149</v>
       </c>
       <c r="E26" s="14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F26" s="24" t="s">
         <v>124</v>
@@ -5199,7 +5196,7 @@
         <v>157</v>
       </c>
       <c r="E27" s="14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F27" s="24" t="s">
         <v>124</v>
@@ -5216,7 +5213,7 @@
         <v>242</v>
       </c>
       <c r="E28" s="14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F28" s="24" t="s">
         <v>124</v>
@@ -5233,7 +5230,7 @@
         <v>155</v>
       </c>
       <c r="E29" s="14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F29" s="24" t="s">
         <v>124</v>
@@ -5250,7 +5247,7 @@
         <v>159</v>
       </c>
       <c r="E30" s="14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F30" s="24" t="s">
         <v>124</v>
@@ -5267,7 +5264,7 @@
         <v>169</v>
       </c>
       <c r="E31" s="14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F31" s="24" t="s">
         <v>124</v>
@@ -5284,7 +5281,7 @@
         <v>238</v>
       </c>
       <c r="E32" s="14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F32" s="24" t="s">
         <v>124</v>
@@ -5301,7 +5298,7 @@
         <v>235</v>
       </c>
       <c r="E33" s="14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F33" s="24" t="s">
         <v>124</v>
@@ -5318,7 +5315,7 @@
         <v>224</v>
       </c>
       <c r="E34" s="14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F34" s="24" t="s">
         <v>124</v>
@@ -5335,7 +5332,7 @@
         <v>250</v>
       </c>
       <c r="E35" s="14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F35" s="24" t="s">
         <v>124</v>
@@ -5352,7 +5349,7 @@
         <v>261</v>
       </c>
       <c r="E36" s="14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F36" s="24" t="s">
         <v>124</v>
@@ -5370,7 +5367,7 @@
         <v>134</v>
       </c>
       <c r="E37" s="14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F37" s="24" t="s">
         <v>124</v>
@@ -5388,7 +5385,7 @@
         <v>136</v>
       </c>
       <c r="E38" s="14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F38" s="24" t="s">
         <v>124</v>
@@ -5406,7 +5403,7 @@
         <v>138</v>
       </c>
       <c r="E39" s="14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F39" s="24" t="s">
         <v>124</v>
@@ -5424,7 +5421,7 @@
         <v>143</v>
       </c>
       <c r="E40" s="14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F40" s="24" t="s">
         <v>124</v>
@@ -5442,7 +5439,7 @@
         <v>145</v>
       </c>
       <c r="E41" s="14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F41" s="24" t="s">
         <v>124</v>
@@ -5460,7 +5457,7 @@
         <v>149</v>
       </c>
       <c r="E42" s="14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F42" s="24" t="s">
         <v>124</v>
@@ -5478,7 +5475,7 @@
         <v>157</v>
       </c>
       <c r="E43" s="14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F43" s="24" t="s">
         <v>124</v>
@@ -5496,7 +5493,7 @@
         <v>242</v>
       </c>
       <c r="E44" s="14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F44" s="24" t="s">
         <v>124</v>
@@ -5514,7 +5511,7 @@
         <v>155</v>
       </c>
       <c r="E45" s="14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F45" s="24" t="s">
         <v>124</v>
@@ -5532,7 +5529,7 @@
         <v>159</v>
       </c>
       <c r="E46" s="14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F46" s="24" t="s">
         <v>124</v>
@@ -5550,7 +5547,7 @@
         <v>169</v>
       </c>
       <c r="E47" s="14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F47" s="24" t="s">
         <v>124</v>
@@ -5568,7 +5565,7 @@
         <v>238</v>
       </c>
       <c r="E48" s="14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F48" s="24" t="s">
         <v>124</v>
@@ -5586,7 +5583,7 @@
         <v>235</v>
       </c>
       <c r="E49" s="14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F49" s="24" t="s">
         <v>124</v>
@@ -5604,7 +5601,7 @@
         <v>224</v>
       </c>
       <c r="E50" s="14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F50" s="24" t="s">
         <v>124</v>
@@ -5622,7 +5619,7 @@
         <v>246</v>
       </c>
       <c r="E51" s="14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F51" s="24" t="s">
         <v>124</v>
@@ -5640,7 +5637,7 @@
         <v>250</v>
       </c>
       <c r="E52" s="14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F52" s="24" t="s">
         <v>124</v>
@@ -5658,7 +5655,7 @@
         <v>261</v>
       </c>
       <c r="E53" s="14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F53" s="24" t="s">
         <v>124</v>
@@ -5768,7 +5765,7 @@
         <v>214</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="G4" s="81" t="s">
         <v>124</v>
@@ -5788,7 +5785,7 @@
         <v>216</v>
       </c>
       <c r="F5" s="14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="G5" s="81" t="s">
         <v>124</v>
@@ -5808,7 +5805,7 @@
         <v>222</v>
       </c>
       <c r="F6" s="14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="G6" s="81" t="s">
         <v>124</v>
@@ -5828,7 +5825,7 @@
         <v>214</v>
       </c>
       <c r="F7" s="14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="G7" s="81" t="s">
         <v>124</v>
@@ -5848,7 +5845,7 @@
         <v>216</v>
       </c>
       <c r="F8" s="14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="G8" s="81" t="s">
         <v>124</v>
@@ -5868,7 +5865,7 @@
         <v>222</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="G9" s="81" t="s">
         <v>124</v>
@@ -5888,7 +5885,7 @@
         <v>214</v>
       </c>
       <c r="F10" s="14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="G10" s="81" t="s">
         <v>124</v>
@@ -5908,7 +5905,7 @@
         <v>216</v>
       </c>
       <c r="F11" s="14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="G11" s="81" t="s">
         <v>124</v>
@@ -5928,7 +5925,7 @@
         <v>222</v>
       </c>
       <c r="F12" s="14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="G12" s="81" t="s">
         <v>124</v>
@@ -5945,7 +5942,7 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.36328125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -6049,7 +6046,7 @@
         <v>234</v>
       </c>
       <c r="F4" s="28" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="I4" t="s">
         <v>117</v>
@@ -6070,7 +6067,7 @@
         <v>234</v>
       </c>
       <c r="F5" s="28" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="I5" s="14" t="s">
         <v>273</v>
@@ -6091,12 +6088,12 @@
         <v>234</v>
       </c>
       <c r="F6" s="28" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="G6" s="14"/>
       <c r="H6" s="14"/>
       <c r="I6" s="14" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
   </sheetData>
@@ -7265,7 +7262,7 @@
       </c>
       <c r="J38" s="28"/>
       <c r="K38" s="28" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="39" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7294,7 +7291,7 @@
       </c>
       <c r="J39" s="28"/>
       <c r="K39" s="28" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="40" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7323,7 +7320,7 @@
       </c>
       <c r="J40" s="28"/>
       <c r="K40" s="28" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="41" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7352,7 +7349,7 @@
       </c>
       <c r="J41" s="28"/>
       <c r="K41" s="28" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="42" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7381,7 +7378,7 @@
       </c>
       <c r="J42" s="28"/>
       <c r="K42" s="28" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="43" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7410,7 +7407,7 @@
       </c>
       <c r="J43" s="28"/>
       <c r="K43" s="28" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="44" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7439,7 +7436,7 @@
       </c>
       <c r="J44" s="28"/>
       <c r="K44" s="28" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="45" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7468,7 +7465,7 @@
       </c>
       <c r="J45" s="28"/>
       <c r="K45" s="28" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="46" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7497,7 +7494,7 @@
       </c>
       <c r="J46" s="28"/>
       <c r="K46" s="28" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="47" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7528,7 +7525,7 @@
       </c>
       <c r="J47" s="28"/>
       <c r="K47" s="28" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="48" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7559,7 +7556,7 @@
       </c>
       <c r="J48" s="28"/>
       <c r="K48" s="28" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="49" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7590,7 +7587,7 @@
       </c>
       <c r="J49" s="28"/>
       <c r="K49" s="28" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="50" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7619,7 +7616,7 @@
       </c>
       <c r="J50" s="28"/>
       <c r="K50" s="28" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="51" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7648,7 +7645,7 @@
       </c>
       <c r="J51" s="28"/>
       <c r="K51" s="28" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="52" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7677,7 +7674,7 @@
       </c>
       <c r="J52" s="28"/>
       <c r="K52" s="28" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="53" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7708,7 +7705,7 @@
       </c>
       <c r="J53" s="28"/>
       <c r="K53" s="28" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="54" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -7737,7 +7734,7 @@
       </c>
       <c r="J54" s="28"/>
       <c r="K54" s="28" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
   </sheetData>
@@ -8008,7 +8005,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+    <sheetView topLeftCell="G1" workbookViewId="0">
       <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
@@ -8155,7 +8152,7 @@
         <v>26</v>
       </c>
       <c r="L4" s="42" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="M4" s="35"/>
       <c r="N4" s="8"/>
@@ -8187,7 +8184,7 @@
         <v>26</v>
       </c>
       <c r="L5" s="42" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="M5" s="35"/>
       <c r="N5" s="8"/>
@@ -8217,7 +8214,7 @@
         <v>26</v>
       </c>
       <c r="L6" s="42" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="7" spans="1:14" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -8247,7 +8244,7 @@
         <v>26</v>
       </c>
       <c r="L7" s="42" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="8" spans="1:14" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -8275,7 +8272,7 @@
         <v>26</v>
       </c>
       <c r="L8" s="42" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
   </sheetData>
@@ -9169,7 +9166,7 @@
         <v>184</v>
       </c>
       <c r="P16" s="14" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="Q16" s="24" t="s">
         <v>73</v>
@@ -9200,7 +9197,7 @@
         <v>185</v>
       </c>
       <c r="P17" s="14" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="Q17" s="24" t="s">
         <v>73</v>
@@ -9231,7 +9228,7 @@
         <v>184</v>
       </c>
       <c r="P18" s="14" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="Q18" s="24" t="s">
         <v>73</v>
@@ -9262,7 +9259,7 @@
         <v>188</v>
       </c>
       <c r="P19" s="14" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="Q19" s="24" t="s">
         <v>73</v>
@@ -9293,7 +9290,7 @@
         <v>199</v>
       </c>
       <c r="P20" s="14" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="Q20" s="24" t="s">
         <v>73</v>
@@ -9324,7 +9321,7 @@
         <v>199</v>
       </c>
       <c r="P21" s="14" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="Q21" s="24" t="s">
         <v>26</v>
@@ -9356,7 +9353,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O134"/>
   <sheetViews>
-    <sheetView topLeftCell="H133" workbookViewId="0">
+    <sheetView topLeftCell="H79" workbookViewId="0">
       <selection activeCell="M127" sqref="M127"/>
     </sheetView>
   </sheetViews>

</xml_diff>